<commit_message>
Chapter 3, 4, 5 and 6
</commit_message>
<xml_diff>
--- a/Planejamento do Curso.xlsx
+++ b/Planejamento do Curso.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e16c958aec6248d8/Documentos/1 - Projects-GitHub/course-node-z/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8B1A722-41D9-48D0-826A-360EE9C0659E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{C8B1A722-41D9-48D0-826A-360EE9C0659E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{557F5626-275F-4FA9-8A36-CB232A5BFF80}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7DF8FB6C-0510-459C-B716-1685F3CBCC9B}"/>
+    <workbookView xWindow="3348" yWindow="348" windowWidth="17280" windowHeight="8880" xr2:uid="{7DF8FB6C-0510-459C-B716-1685F3CBCC9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Introduction</t>
   </si>
@@ -105,13 +105,16 @@
   </si>
   <si>
     <t>DIAS</t>
+  </si>
+  <si>
+    <t>NODE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,13 +129,33 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,15 +170,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -176,16 +202,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -197,6 +213,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -496,149 +516,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B30B61-502C-46A2-9BA1-0A0E5A49AB28}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="1" max="1" width="49.88671875" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45297</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45298</v>
+      </c>
+      <c r="C4">
+        <f>B4-B3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" s="2">
+        <v>45299</v>
+      </c>
+      <c r="C5">
+        <f>B5-B4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45300</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C22" si="0">B6-B5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45301</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <f ca="1">TODAY()</f>
+        <v>45301</v>
+      </c>
+      <c r="G7">
+        <f ca="1">F8-F7</f>
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>45298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2">
-        <f ca="1">TODAY()</f>
-        <v>45298</v>
-      </c>
-      <c r="G6">
-        <f ca="1">F7-F6</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-45301</v>
+      </c>
+      <c r="F8" s="2">
         <v>45322</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G6">
+  <conditionalFormatting sqref="G7">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -647,5 +763,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
planet project for Node.js
</commit_message>
<xml_diff>
--- a/Planejamento do Curso.xlsx
+++ b/Planejamento do Curso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e16c958aec6248d8/Documentos/1 - Projects-GitHub/course-node-z/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{C8B1A722-41D9-48D0-826A-360EE9C0659E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{557F5626-275F-4FA9-8A36-CB232A5BFF80}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{C8B1A722-41D9-48D0-826A-360EE9C0659E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74ADE6B5-21C7-4748-B796-4073C8C2B745}"/>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="348" windowWidth="17280" windowHeight="8880" xr2:uid="{7DF8FB6C-0510-459C-B716-1685F3CBCC9B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7DF8FB6C-0510-459C-B716-1685F3CBCC9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Introduction</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>NODE</t>
+  </si>
+  <si>
+    <t>META</t>
   </si>
 </sst>
 </file>
@@ -519,13 +522,14 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="49.88671875" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -544,6 +548,9 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -605,11 +612,11 @@
       </c>
       <c r="F7" s="2">
         <f ca="1">TODAY()</f>
-        <v>45301</v>
+        <v>45305</v>
       </c>
       <c r="G7">
         <f ca="1">F8-F7</f>
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -620,6 +627,9 @@
         <f t="shared" si="0"/>
         <v>-45301</v>
       </c>
+      <c r="D8" s="2">
+        <v>45302</v>
+      </c>
       <c r="F8" s="2">
         <v>45322</v>
       </c>
@@ -632,6 +642,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D9" s="2">
+        <v>45303</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -641,6 +654,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D10" s="2">
+        <v>45304</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -649,6 +665,9 @@
       <c r="C11">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45305</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>